<commit_message>
Data and Keyword Driven Framework notes and programs till Mar 2th
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excels/MasterTestData.xlsx
+++ b/src/test/resources/testdata/excels/MasterTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FLM5thDecWS\DataAndKeywordDrivenFramework\src\test\resources\testdata\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF1043B-BAF4-4EAE-98E9-16F7FDEC6864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A6CB02-D01F-4C16-B815-90A99A652C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8AC35321-73B4-4C70-8779-555AFECB24AD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>TC-001</t>
   </si>
@@ -64,13 +64,46 @@
   </si>
   <si>
     <t>Adactin.com - Hotel Reservation System</t>
+  </si>
+  <si>
+    <t>TC-003</t>
+  </si>
+  <si>
+    <t>kiran2403</t>
+  </si>
+  <si>
+    <t>kiran123</t>
+  </si>
+  <si>
+    <t>confirm Password</t>
+  </si>
+  <si>
+    <t>Full  Name</t>
+  </si>
+  <si>
+    <t>email id</t>
+  </si>
+  <si>
+    <t>captcha</t>
+  </si>
+  <si>
+    <t>Kiran Kumar</t>
+  </si>
+  <si>
+    <t>abcd@gmail.com</t>
+  </si>
+  <si>
+    <t>Hyderabad</t>
+  </si>
+  <si>
+    <t>Adactin.com - New User Registration</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +124,14 @@
       <name val="Comic Sans MS"/>
       <family val="4"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -109,15 +150,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -430,22 +474,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D115DE3-8673-48E1-AB0E-9020206768B9}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="50.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,7 +507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -473,7 +521,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -487,7 +535,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -501,7 +549,62 @@
         <v>9</v>
       </c>
     </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G8" r:id="rId1" xr:uid="{C46CB3C7-FF13-4EC7-93C2-2D702C31325F}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Java programs with soultuion added
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/excels/MasterTestData.xlsx
+++ b/src/test/resources/testdata/excels/MasterTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FLM5thDecWS\DataAndKeywordDrivenFramework\src\test\resources\testdata\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A6CB02-D01F-4C16-B815-90A99A652C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A0AC534-D019-4DDE-AA6C-0F03BF92A9D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8AC35321-73B4-4C70-8779-555AFECB24AD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>TC-001</t>
   </si>
@@ -97,6 +97,18 @@
   </si>
   <si>
     <t>Adactin.com - New User Registration</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>TC-004</t>
+  </si>
+  <si>
+    <t>errorMessage</t>
+  </si>
+  <si>
+    <t>Enter Username</t>
   </si>
 </sst>
 </file>
@@ -474,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D115DE3-8673-48E1-AB0E-9020206768B9}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
@@ -601,6 +613,27 @@
         <v>19</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G8" r:id="rId1" xr:uid="{C46CB3C7-FF13-4EC7-93C2-2D702C31325F}"/>

</xml_diff>